<commit_message>
Update Figure 5 bar chart Excel files
Revised the data in Fig5a_pregnancy_PB_bar.xlsx, Fig5b_lactation_PB_bar.xlsx, and Fig5c_PW_PB_bar.xlsx to reflect updated results or corrections for Figure 5.
</commit_message>
<xml_diff>
--- a/Figure5/Fig5a_pregnancy_PB_bar.xlsx
+++ b/Figure5/Fig5a_pregnancy_PB_bar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murrell\OneDrive - Washington University in St. Louis\Documents\Github\Ghrelinpaper\Murrell2025\Figure5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gowustl-my.sharepoint.com/personal/murrell_wustl_edu/Documents/Documents/Github/Ghrelinpaper/Murrell2025/Figure5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD6E5A41-94F0-4899-A224-E8913A779603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{CD6E5A41-94F0-4899-A224-E8913A779603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FA32A41-4B4A-4B98-99A9-8A90EF1B1DF7}"/>
   <bookViews>
-    <workbookView xWindow="35865" yWindow="1350" windowWidth="20895" windowHeight="13905" xr2:uid="{0E135258-AB9E-460A-922C-0B7CC504210E}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="26880" windowHeight="11295" xr2:uid="{0E135258-AB9E-460A-922C-0B7CC504210E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Baseline</t>
   </si>
   <si>
-    <t>Anticipitory</t>
-  </si>
-  <si>
     <t>PB</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>P15_mouse8</t>
+  </si>
+  <si>
+    <t>Anticipatory</t>
   </si>
 </sst>
 </file>
@@ -508,86 +508,86 @@
   <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>16</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>21</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>22</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>23</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>24</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>25</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>26</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
@@ -669,7 +669,7 @@
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1">
         <v>-0.94800114700000004</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="1">
         <v>-1.6579270770000001</v>

</xml_diff>